<commit_message>
get Preference Share Capital % value from label added.
</commit_message>
<xml_diff>
--- a/uploads/1680591417855-FCFE Input Sheet with Formula (1).xlsx
+++ b/uploads/1680591417855-FCFE Input Sheet with Formula (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ifinworth\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A4F0FE-FB08-42BE-9848-F3C485C6A9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AC26DA-4751-4476-9469-8BCE57419333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11B12A5D-7249-4041-8AA7-3E354D49454B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{11B12A5D-7249-4041-8AA7-3E354D49454B}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;L" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
     <t>Equity Share Capital</t>
   </si>
   <si>
-    <t>Preference Share Capital</t>
-  </si>
-  <si>
     <t>Other Equity</t>
   </si>
   <si>
@@ -568,6 +565,9 @@
   </si>
   <si>
     <t>Provisionals/Audited Nos. close to valuation 2022-2023</t>
+  </si>
+  <si>
+    <t>60 % Preference Share Capital</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D100AD-1EC3-3246-AFE5-16D06F619914}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1360,28 +1360,28 @@
   <sheetData>
     <row r="1" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B1" s="79" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C1" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="77" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="E1" s="77" t="s">
         <v>173</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="F1" s="77" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="G1" s="77" t="s">
         <v>175</v>
       </c>
-      <c r="G1" s="77" t="s">
-        <v>176</v>
-      </c>
       <c r="J1" s="50" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1433,7 +1433,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" s="5">
         <v>221221361</v>
@@ -1537,7 +1537,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C13" s="35" t="e">
         <f>+B13*1.03</f>
@@ -1822,7 +1822,7 @@
         <v>18</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" s="29">
         <v>0</v>
@@ -1867,7 +1867,7 @@
         <v>20</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C31" s="29">
         <v>0</v>
@@ -1912,7 +1912,7 @@
         <v>22</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C33" s="29">
         <v>0</v>
@@ -2004,7 +2004,7 @@
         <v>26</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C37" s="33">
         <v>0</v>
@@ -2025,7 +2025,7 @@
         <v>27</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C38" s="33">
         <v>0</v>
@@ -2046,7 +2046,7 @@
         <v>28</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C39" s="33">
         <v>0</v>
@@ -2067,7 +2067,7 @@
         <v>29</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C40" s="33">
         <v>0</v>
@@ -2141,7 +2141,7 @@
         <v>32</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C45" s="33">
         <v>0</v>
@@ -2162,7 +2162,7 @@
         <v>33</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C46" s="33">
         <v>0</v>
@@ -2192,7 +2192,7 @@
         <v>34</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C48" s="33">
         <v>0</v>
@@ -2213,7 +2213,7 @@
         <v>35</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C49" s="33">
         <v>0</v>
@@ -2234,7 +2234,7 @@
         <v>36</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C50" s="33">
         <v>0</v>
@@ -2264,7 +2264,7 @@
         <v>37</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C52" s="33">
         <v>0</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B55" s="46"/>
       <c r="C55" s="7"/>
@@ -2326,7 +2326,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B56" s="46"/>
       <c r="C56" s="7"/>
@@ -2337,7 +2337,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B57" s="46"/>
       <c r="C57" s="7"/>
@@ -2348,7 +2348,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="46" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B58" s="48" t="e">
         <v>#VALUE!</v>
@@ -2368,7 +2368,7 @@
       </c>
       <c r="G58" s="7"/>
       <c r="J58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2389,8 +2389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABB34C2-FC5D-EB4C-A739-CF87FCBB2D79}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2402,25 +2402,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="80" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="77" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C1" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="77" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="E1" s="77" t="s">
         <v>173</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="F1" s="77" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="G1" s="77" t="s">
         <v>175</v>
-      </c>
-      <c r="G1" s="77" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2515,7 +2515,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="54" t="s">
-        <v>42</v>
+        <v>178</v>
       </c>
       <c r="B8" s="26">
         <v>0</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="26">
         <v>0</v>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="26">
         <v>0</v>
@@ -2578,7 +2578,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="54" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="26">
         <v>76000758</v>
@@ -2601,7 +2601,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="26">
         <v>0</v>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="26">
         <v>0</v>
@@ -2643,7 +2643,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="26">
         <v>0</v>
@@ -2664,7 +2664,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
@@ -2675,7 +2675,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="26">
         <v>0</v>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="26">
         <v>0</v>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="26">
         <v>0</v>
@@ -2762,7 +2762,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
@@ -2773,7 +2773,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="26">
         <v>0</v>
@@ -2817,7 +2817,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="26">
         <f>SUM(B25:B31)</f>
@@ -2846,7 +2846,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="26">
         <v>0</v>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" s="2">
         <v>147115025.78</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
@@ -2924,7 +2924,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="26">
         <v>0</v>
@@ -2947,7 +2947,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="26">
         <v>0</v>
@@ -2968,7 +2968,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B31" s="26">
         <v>0</v>
@@ -2998,7 +2998,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="57">
         <f>SUM(B34:B40)</f>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="26">
         <v>131314212</v>
@@ -3050,7 +3050,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="26">
         <v>0</v>
@@ -3071,7 +3071,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B36" s="3">
         <v>17180255.309999999</v>
@@ -3094,7 +3094,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B37" s="26">
         <v>0</v>
@@ -3115,7 +3115,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" s="26">
         <v>311380626.45999998</v>
@@ -3138,7 +3138,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" s="1">
         <v>19755608</v>
@@ -3166,7 +3166,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40" s="57"/>
       <c r="C40" s="57"/>
@@ -3177,7 +3177,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B41" s="57">
         <f>+B33+B27+B6</f>
@@ -3215,7 +3215,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B43" s="57"/>
       <c r="C43" s="57"/>
@@ -3235,7 +3235,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B45" s="57">
         <f>+B46+SUM(B55:B59)</f>
@@ -3264,7 +3264,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B46" s="26">
         <f>SUM(B48:B53)</f>
@@ -3293,7 +3293,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B47" s="26"/>
       <c r="C47" s="26"/>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" s="26">
         <v>342570791</v>
@@ -3327,7 +3327,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B49" s="26">
         <v>0</v>
@@ -3348,7 +3348,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B50" s="26">
         <v>0</v>
@@ -3369,7 +3369,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B51" s="26">
         <v>0</v>
@@ -3390,7 +3390,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B52" s="26">
         <v>0</v>
@@ -3411,7 +3411,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B53" s="26">
         <v>0</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B55" s="26">
         <v>0</v>
@@ -3462,7 +3462,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B56" s="1">
         <v>29770092</v>
@@ -3485,7 +3485,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B57" s="26">
         <v>0</v>
@@ -3506,7 +3506,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B58" s="26">
         <v>92251687</v>
@@ -3529,7 +3529,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B59" s="4">
         <v>1796625</v>
@@ -3566,7 +3566,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B61" s="26">
         <f>SUM(B62:B69)</f>
@@ -3595,7 +3595,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B62" s="26">
         <v>6053565</v>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B63" s="26">
         <v>0</v>
@@ -3639,7 +3639,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B64" s="13">
         <v>42700049</v>
@@ -3662,7 +3662,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B65" s="13">
         <v>0</v>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B66" s="13">
         <v>115000000</v>
@@ -3706,7 +3706,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="61" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B67" s="13">
         <v>87608143</v>
@@ -3729,7 +3729,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B68" s="13">
         <v>0</v>
@@ -3750,7 +3750,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B69" s="15">
         <v>18795533</v>
@@ -3796,7 +3796,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" s="57">
         <f>+B45+B61</f>
@@ -3864,38 +3864,38 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="82" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="17"/>
       <c r="D1" s="74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="69" t="s">
         <v>97</v>
-      </c>
-      <c r="B3" s="69" t="s">
-        <v>98</v>
       </c>
       <c r="C3" s="62"/>
       <c r="D3" s="75" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>100</v>
       </c>
       <c r="C4" s="63"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" s="70">
         <f>+'P&amp;L'!B42</f>
@@ -3903,15 +3903,15 @@
       </c>
       <c r="C5" s="64"/>
       <c r="D5" s="75" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6" s="70">
         <f>+'P&amp;L'!B26</f>
@@ -3919,12 +3919,12 @@
       </c>
       <c r="C6" s="64"/>
       <c r="D6" s="75" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="70" t="e">
         <f>+(-'P&amp;L'!B29+'P&amp;L'!B31+'P&amp;L'!B33)</f>
@@ -3932,22 +3932,22 @@
       </c>
       <c r="C7" s="64"/>
       <c r="D7" s="75" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G7" s="81" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H7" s="81"/>
       <c r="I7" s="81"/>
       <c r="K7" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L7" s="83"/>
       <c r="M7" s="83"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="70" t="e">
         <f>+(SUM(_xlfn.SINGLE(BS!B64:B69)-BS!B68)-SUM(BS!B34:B40))-(SUM(_xlfn.SINGLE(BS!#REF!)-BS!#REF!)-SUM(BS!#REF!))</f>
@@ -3955,24 +3955,24 @@
       </c>
       <c r="C8" s="64"/>
       <c r="D8" s="75" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K8" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="M8" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="L8" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9" s="70" t="e">
         <f>+(BS!B59-BS!B25)-(BS!#REF!-BS!#REF!)</f>
@@ -3980,24 +3980,24 @@
       </c>
       <c r="C9" s="64"/>
       <c r="D9" s="75" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="68" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="71" t="e">
         <f>+B5+B6+B7+B8+B9</f>
@@ -4005,21 +4005,21 @@
       </c>
       <c r="C10" s="65"/>
       <c r="D10" s="75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="70" t="e">
         <f>+BS!B46-BS!#REF!</f>
@@ -4027,18 +4027,18 @@
       </c>
       <c r="C11" s="64"/>
       <c r="D11" s="75" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="72" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="73" t="e">
         <f>B10+B11</f>
@@ -4046,68 +4046,68 @@
       </c>
       <c r="C12" s="66"/>
       <c r="D12" s="76" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="D13" s="75" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="7" t="e">
         <f>1/(1+[1]Sheet2!C20)^B13</f>
         <v>#VALUE!</v>
       </c>
       <c r="D14" s="74" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="E14" s="50" t="s">
-        <v>141</v>
-      </c>
       <c r="I14" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15" s="7" t="e">
         <f>+B14*B12</f>
         <v>#VALUE!</v>
       </c>
       <c r="D15" s="75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B16" s="8" t="e">
         <f>SUM(B15:H15)</f>
@@ -4115,15 +4115,15 @@
       </c>
       <c r="C16" s="67"/>
       <c r="D16" s="75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17" s="8">
         <f>+BS!B27</f>
@@ -4131,64 +4131,64 @@
       </c>
       <c r="C17" s="67"/>
       <c r="D17" s="75" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B18" s="7">
         <f>+BS!B62+BS!B63</f>
         <v>6053565</v>
       </c>
       <c r="D18" s="75" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B19" s="7">
         <f>+BS!B56+BS!B68</f>
         <v>29770092</v>
       </c>
       <c r="D19" s="75" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>117</v>
-      </c>
       <c r="D20" s="75" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G20" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="I20" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="I20" s="19" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B21" s="9" t="e">
         <f>+B16-B17+B18+B19+B20</f>
@@ -4196,24 +4196,24 @@
       </c>
       <c r="C21" s="63"/>
       <c r="D21" s="75" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B22" s="7" t="str">
         <f>+[1]Sheet2!C11</f>
         <v>Ask user for same</v>
       </c>
       <c r="D22" s="75" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23" s="9" t="e">
         <f>+B21/B22</f>
@@ -4221,41 +4221,41 @@
       </c>
       <c r="C23" s="63"/>
       <c r="D23" s="76" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G23" s="81" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H23" s="81"/>
       <c r="I23" s="81"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G24" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24" s="10" t="s">
         <v>153</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G27" s="81" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H27" s="81"/>
       <c r="I27" s="81"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G28" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="I28" s="12" t="s">
         <v>156</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>